<commit_message>
new file:   gradetask/createpdfs.sh 	modified:   gradetask/gradetask 	deleted:    gradetask/job.sh 	modified:   gradetask/main.go 	renamed:    gradetask/templ.tex -> gradetask/templ.tex.tpl 	modified:   "gradetask/\346\257\225\350\256\276\347\231\273\350\256\260\350\241\250.xlsx"
</commit_message>
<xml_diff>
--- a/gradetask/毕设登记表.xlsx
+++ b/gradetask/毕设登记表.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\docs\教学\2017-2018-2\毕业设计相关工作\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -684,10 +684,6 @@
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
   <si>
-    <t>守一大厦建筑设计</t>
-    <phoneticPr fontId="5" type="noConversion"/>
-  </si>
-  <si>
     <t>福州市仓山区新生活疗养院办公楼设计</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
@@ -705,6 +701,10 @@
   </si>
   <si>
     <t>福州市晋安区静姝疗养院办公楼设计</t>
+    <phoneticPr fontId="5" type="noConversion"/>
+  </si>
+  <si>
+    <t>守一大厦设计</t>
     <phoneticPr fontId="5" type="noConversion"/>
   </si>
 </sst>
@@ -2001,65 +2001,65 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="32" fillId="10" borderId="10" xfId="73" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="10" borderId="10" xfId="73" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="10" borderId="10" xfId="73" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="10" borderId="10" xfId="73" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="128">
@@ -2492,7 +2492,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
@@ -2513,202 +2513,202 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="122" t="s">
+      <c r="A1" s="111" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="122"/>
-      <c r="C1" s="122"/>
-      <c r="D1" s="122"/>
-      <c r="E1" s="122"/>
-      <c r="F1" s="122"/>
-      <c r="G1" s="122"/>
-      <c r="H1" s="122"/>
-      <c r="I1" s="122"/>
-      <c r="J1" s="122"/>
-      <c r="K1" s="122"/>
-      <c r="L1" s="122"/>
-      <c r="M1" s="122"/>
-      <c r="N1" s="122"/>
-      <c r="O1" s="122"/>
-      <c r="P1" s="122"/>
-      <c r="Q1" s="122"/>
+      <c r="B1" s="111"/>
+      <c r="C1" s="111"/>
+      <c r="D1" s="111"/>
+      <c r="E1" s="111"/>
+      <c r="F1" s="111"/>
+      <c r="G1" s="111"/>
+      <c r="H1" s="111"/>
+      <c r="I1" s="111"/>
+      <c r="J1" s="111"/>
+      <c r="K1" s="111"/>
+      <c r="L1" s="111"/>
+      <c r="M1" s="111"/>
+      <c r="N1" s="111"/>
+      <c r="O1" s="111"/>
+      <c r="P1" s="111"/>
+      <c r="Q1" s="111"/>
     </row>
     <row r="2" spans="1:18" ht="18.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="122" t="s">
+      <c r="A2" s="111" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="122"/>
-      <c r="C2" s="122"/>
-      <c r="D2" s="122"/>
-      <c r="E2" s="122"/>
-      <c r="F2" s="122"/>
-      <c r="G2" s="122"/>
-      <c r="H2" s="122"/>
-      <c r="I2" s="122"/>
-      <c r="J2" s="122"/>
-      <c r="K2" s="122"/>
-      <c r="L2" s="122"/>
-      <c r="M2" s="122"/>
-      <c r="N2" s="122"/>
-      <c r="O2" s="122"/>
-      <c r="P2" s="122"/>
-      <c r="Q2" s="122"/>
+      <c r="B2" s="111"/>
+      <c r="C2" s="111"/>
+      <c r="D2" s="111"/>
+      <c r="E2" s="111"/>
+      <c r="F2" s="111"/>
+      <c r="G2" s="111"/>
+      <c r="H2" s="111"/>
+      <c r="I2" s="111"/>
+      <c r="J2" s="111"/>
+      <c r="K2" s="111"/>
+      <c r="L2" s="111"/>
+      <c r="M2" s="111"/>
+      <c r="N2" s="111"/>
+      <c r="O2" s="111"/>
+      <c r="P2" s="111"/>
+      <c r="Q2" s="111"/>
     </row>
     <row r="3" spans="1:18" ht="16.2" x14ac:dyDescent="0.3">
-      <c r="A3" s="123" t="s">
+      <c r="A3" s="112" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="123"/>
-      <c r="C3" s="123"/>
-      <c r="D3" s="123"/>
-      <c r="E3" s="123"/>
-      <c r="F3" s="123"/>
-      <c r="G3" s="123"/>
-      <c r="H3" s="123"/>
-      <c r="I3" s="123"/>
-      <c r="J3" s="123"/>
-      <c r="K3" s="123"/>
-      <c r="L3" s="123"/>
-      <c r="M3" s="123"/>
-      <c r="N3" s="123"/>
-      <c r="O3" s="123"/>
-      <c r="P3" s="123"/>
-      <c r="Q3" s="123"/>
+      <c r="B3" s="112"/>
+      <c r="C3" s="112"/>
+      <c r="D3" s="112"/>
+      <c r="E3" s="112"/>
+      <c r="F3" s="112"/>
+      <c r="G3" s="112"/>
+      <c r="H3" s="112"/>
+      <c r="I3" s="112"/>
+      <c r="J3" s="112"/>
+      <c r="K3" s="112"/>
+      <c r="L3" s="112"/>
+      <c r="M3" s="112"/>
+      <c r="N3" s="112"/>
+      <c r="O3" s="112"/>
+      <c r="P3" s="112"/>
+      <c r="Q3" s="112"/>
     </row>
     <row r="4" spans="1:18" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="113" t="s">
+      <c r="A4" s="116" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="113" t="s">
+      <c r="B4" s="116" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="124" t="s">
+      <c r="C4" s="113" t="s">
         <v>5</v>
       </c>
-      <c r="D4" s="125"/>
-      <c r="E4" s="124" t="s">
+      <c r="D4" s="114"/>
+      <c r="E4" s="113" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="126"/>
-      <c r="G4" s="126"/>
-      <c r="H4" s="126"/>
-      <c r="I4" s="125"/>
-      <c r="J4" s="124" t="s">
+      <c r="F4" s="115"/>
+      <c r="G4" s="115"/>
+      <c r="H4" s="115"/>
+      <c r="I4" s="114"/>
+      <c r="J4" s="113" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="125"/>
-      <c r="L4" s="113" t="s">
+      <c r="K4" s="114"/>
+      <c r="L4" s="116" t="s">
         <v>8</v>
       </c>
-      <c r="M4" s="113" t="s">
+      <c r="M4" s="116" t="s">
         <v>9</v>
       </c>
-      <c r="N4" s="118" t="s">
+      <c r="N4" s="125" t="s">
         <v>10</v>
       </c>
-      <c r="O4" s="113" t="s">
+      <c r="O4" s="116" t="s">
         <v>11</v>
       </c>
-      <c r="P4" s="113" t="s">
+      <c r="P4" s="116" t="s">
         <v>12</v>
       </c>
-      <c r="Q4" s="113" t="s">
+      <c r="Q4" s="116" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:18" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="111"/>
-      <c r="B5" s="116"/>
-      <c r="C5" s="110" t="s">
+      <c r="A5" s="117"/>
+      <c r="B5" s="119"/>
+      <c r="C5" s="121" t="s">
         <v>14</v>
       </c>
-      <c r="D5" s="110" t="s">
+      <c r="D5" s="121" t="s">
         <v>15</v>
       </c>
-      <c r="E5" s="110" t="s">
+      <c r="E5" s="121" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="110" t="s">
+      <c r="F5" s="121" t="s">
         <v>17</v>
       </c>
-      <c r="G5" s="110" t="s">
+      <c r="G5" s="121" t="s">
         <v>18</v>
       </c>
-      <c r="H5" s="110" t="s">
+      <c r="H5" s="121" t="s">
         <v>19</v>
       </c>
-      <c r="I5" s="110" t="s">
+      <c r="I5" s="121" t="s">
         <v>20</v>
       </c>
-      <c r="J5" s="110" t="s">
+      <c r="J5" s="121" t="s">
         <v>21</v>
       </c>
-      <c r="K5" s="110" t="s">
+      <c r="K5" s="121" t="s">
         <v>22</v>
       </c>
-      <c r="L5" s="111"/>
-      <c r="M5" s="116"/>
-      <c r="N5" s="119"/>
-      <c r="O5" s="116"/>
-      <c r="P5" s="111"/>
-      <c r="Q5" s="111"/>
+      <c r="L5" s="117"/>
+      <c r="M5" s="119"/>
+      <c r="N5" s="126"/>
+      <c r="O5" s="119"/>
+      <c r="P5" s="117"/>
+      <c r="Q5" s="117"/>
     </row>
     <row r="6" spans="1:18" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="111"/>
-      <c r="B6" s="116"/>
-      <c r="C6" s="111"/>
-      <c r="D6" s="111"/>
-      <c r="E6" s="111"/>
-      <c r="F6" s="111"/>
-      <c r="G6" s="111"/>
-      <c r="H6" s="111"/>
-      <c r="I6" s="111"/>
-      <c r="J6" s="111"/>
-      <c r="K6" s="111"/>
-      <c r="L6" s="111"/>
-      <c r="M6" s="116"/>
-      <c r="N6" s="119"/>
-      <c r="O6" s="116"/>
-      <c r="P6" s="111"/>
-      <c r="Q6" s="111"/>
+      <c r="A6" s="117"/>
+      <c r="B6" s="119"/>
+      <c r="C6" s="117"/>
+      <c r="D6" s="117"/>
+      <c r="E6" s="117"/>
+      <c r="F6" s="117"/>
+      <c r="G6" s="117"/>
+      <c r="H6" s="117"/>
+      <c r="I6" s="117"/>
+      <c r="J6" s="117"/>
+      <c r="K6" s="117"/>
+      <c r="L6" s="117"/>
+      <c r="M6" s="119"/>
+      <c r="N6" s="126"/>
+      <c r="O6" s="119"/>
+      <c r="P6" s="117"/>
+      <c r="Q6" s="117"/>
     </row>
     <row r="7" spans="1:18" s="1" customFormat="1" ht="12" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="111"/>
-      <c r="B7" s="116"/>
-      <c r="C7" s="111"/>
-      <c r="D7" s="111"/>
-      <c r="E7" s="111"/>
-      <c r="F7" s="111"/>
-      <c r="G7" s="111"/>
-      <c r="H7" s="111"/>
-      <c r="I7" s="111"/>
-      <c r="J7" s="111"/>
-      <c r="K7" s="111"/>
-      <c r="L7" s="111"/>
-      <c r="M7" s="116"/>
-      <c r="N7" s="119"/>
-      <c r="O7" s="116"/>
-      <c r="P7" s="111"/>
-      <c r="Q7" s="111"/>
+      <c r="A7" s="117"/>
+      <c r="B7" s="119"/>
+      <c r="C7" s="117"/>
+      <c r="D7" s="117"/>
+      <c r="E7" s="117"/>
+      <c r="F7" s="117"/>
+      <c r="G7" s="117"/>
+      <c r="H7" s="117"/>
+      <c r="I7" s="117"/>
+      <c r="J7" s="117"/>
+      <c r="K7" s="117"/>
+      <c r="L7" s="117"/>
+      <c r="M7" s="119"/>
+      <c r="N7" s="126"/>
+      <c r="O7" s="119"/>
+      <c r="P7" s="117"/>
+      <c r="Q7" s="117"/>
     </row>
     <row r="8" spans="1:18" s="1" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="112"/>
-      <c r="B8" s="117"/>
-      <c r="C8" s="112"/>
-      <c r="D8" s="112"/>
-      <c r="E8" s="112"/>
-      <c r="F8" s="112"/>
-      <c r="G8" s="112"/>
-      <c r="H8" s="112"/>
-      <c r="I8" s="112"/>
-      <c r="J8" s="112"/>
-      <c r="K8" s="112"/>
-      <c r="L8" s="112"/>
-      <c r="M8" s="117"/>
-      <c r="N8" s="120"/>
-      <c r="O8" s="117"/>
-      <c r="P8" s="112"/>
-      <c r="Q8" s="112"/>
+      <c r="A8" s="118"/>
+      <c r="B8" s="120"/>
+      <c r="C8" s="118"/>
+      <c r="D8" s="118"/>
+      <c r="E8" s="118"/>
+      <c r="F8" s="118"/>
+      <c r="G8" s="118"/>
+      <c r="H8" s="118"/>
+      <c r="I8" s="118"/>
+      <c r="J8" s="118"/>
+      <c r="K8" s="118"/>
+      <c r="L8" s="118"/>
+      <c r="M8" s="120"/>
+      <c r="N8" s="127"/>
+      <c r="O8" s="120"/>
+      <c r="P8" s="118"/>
+      <c r="Q8" s="118"/>
     </row>
     <row r="9" spans="1:18" ht="25.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
@@ -2961,7 +2961,7 @@
         <v>7</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>188</v>
+        <v>193</v>
       </c>
       <c r="C15" s="98" t="s">
         <v>168</v>
@@ -3004,8 +3004,8 @@
       <c r="A16" s="8">
         <v>8</v>
       </c>
-      <c r="B16" s="127" t="s">
-        <v>189</v>
+      <c r="B16" s="108" t="s">
+        <v>188</v>
       </c>
       <c r="C16" s="98" t="s">
         <v>168</v>
@@ -3048,8 +3048,8 @@
       <c r="A17" s="8">
         <v>9</v>
       </c>
-      <c r="B17" s="128" t="s">
-        <v>190</v>
+      <c r="B17" s="109" t="s">
+        <v>189</v>
       </c>
       <c r="C17" s="98" t="s">
         <v>168</v>
@@ -3092,8 +3092,8 @@
       <c r="A18" s="8">
         <v>10</v>
       </c>
-      <c r="B18" s="127" t="s">
-        <v>191</v>
+      <c r="B18" s="108" t="s">
+        <v>190</v>
       </c>
       <c r="C18" s="98" t="s">
         <v>168</v>
@@ -3136,8 +3136,8 @@
       <c r="A19" s="8">
         <v>11</v>
       </c>
-      <c r="B19" s="129" t="s">
-        <v>192</v>
+      <c r="B19" s="110" t="s">
+        <v>191</v>
       </c>
       <c r="C19" s="98" t="s">
         <v>168</v>
@@ -3180,8 +3180,8 @@
       <c r="A20" s="8">
         <v>12</v>
       </c>
-      <c r="B20" s="129" t="s">
-        <v>193</v>
+      <c r="B20" s="110" t="s">
+        <v>192</v>
       </c>
       <c r="C20" s="98" t="s">
         <v>168</v>
@@ -4691,107 +4691,107 @@
       <c r="Q68" s="19"/>
     </row>
     <row r="69" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A69" s="121" t="s">
+      <c r="A69" s="128" t="s">
         <v>162</v>
       </c>
-      <c r="B69" s="121"/>
-      <c r="C69" s="121"/>
-      <c r="D69" s="121"/>
-      <c r="E69" s="121"/>
-      <c r="F69" s="121"/>
-      <c r="G69" s="121"/>
-      <c r="H69" s="121"/>
-      <c r="I69" s="121"/>
-      <c r="J69" s="121"/>
-      <c r="K69" s="121"/>
-      <c r="L69" s="121"/>
-      <c r="M69" s="121"/>
-      <c r="N69" s="121"/>
-      <c r="O69" s="121"/>
-      <c r="P69" s="114"/>
-      <c r="Q69" s="114"/>
+      <c r="B69" s="128"/>
+      <c r="C69" s="128"/>
+      <c r="D69" s="128"/>
+      <c r="E69" s="128"/>
+      <c r="F69" s="128"/>
+      <c r="G69" s="128"/>
+      <c r="H69" s="128"/>
+      <c r="I69" s="128"/>
+      <c r="J69" s="128"/>
+      <c r="K69" s="128"/>
+      <c r="L69" s="128"/>
+      <c r="M69" s="128"/>
+      <c r="N69" s="128"/>
+      <c r="O69" s="128"/>
+      <c r="P69" s="123"/>
+      <c r="Q69" s="123"/>
     </row>
     <row r="70" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A70" s="108" t="s">
+      <c r="A70" s="122" t="s">
         <v>163</v>
       </c>
-      <c r="B70" s="108"/>
-      <c r="C70" s="108"/>
-      <c r="D70" s="108"/>
-      <c r="E70" s="108"/>
-      <c r="F70" s="108"/>
-      <c r="G70" s="108"/>
-      <c r="H70" s="108"/>
-      <c r="I70" s="108"/>
-      <c r="J70" s="108"/>
-      <c r="K70" s="108"/>
-      <c r="L70" s="108"/>
-      <c r="M70" s="108"/>
-      <c r="N70" s="108"/>
-      <c r="O70" s="108"/>
-      <c r="P70" s="115"/>
-      <c r="Q70" s="115"/>
+      <c r="B70" s="122"/>
+      <c r="C70" s="122"/>
+      <c r="D70" s="122"/>
+      <c r="E70" s="122"/>
+      <c r="F70" s="122"/>
+      <c r="G70" s="122"/>
+      <c r="H70" s="122"/>
+      <c r="I70" s="122"/>
+      <c r="J70" s="122"/>
+      <c r="K70" s="122"/>
+      <c r="L70" s="122"/>
+      <c r="M70" s="122"/>
+      <c r="N70" s="122"/>
+      <c r="O70" s="122"/>
+      <c r="P70" s="124"/>
+      <c r="Q70" s="124"/>
     </row>
     <row r="71" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A71" s="109" t="s">
+      <c r="A71" s="129" t="s">
         <v>164</v>
       </c>
-      <c r="B71" s="109"/>
-      <c r="C71" s="109"/>
-      <c r="D71" s="109"/>
-      <c r="E71" s="109"/>
-      <c r="F71" s="109"/>
-      <c r="G71" s="109"/>
-      <c r="H71" s="109"/>
-      <c r="I71" s="109"/>
-      <c r="J71" s="109"/>
-      <c r="K71" s="109"/>
-      <c r="L71" s="109"/>
-      <c r="M71" s="109"/>
-      <c r="N71" s="109"/>
-      <c r="O71" s="109"/>
-      <c r="P71" s="115"/>
-      <c r="Q71" s="115"/>
+      <c r="B71" s="129"/>
+      <c r="C71" s="129"/>
+      <c r="D71" s="129"/>
+      <c r="E71" s="129"/>
+      <c r="F71" s="129"/>
+      <c r="G71" s="129"/>
+      <c r="H71" s="129"/>
+      <c r="I71" s="129"/>
+      <c r="J71" s="129"/>
+      <c r="K71" s="129"/>
+      <c r="L71" s="129"/>
+      <c r="M71" s="129"/>
+      <c r="N71" s="129"/>
+      <c r="O71" s="129"/>
+      <c r="P71" s="124"/>
+      <c r="Q71" s="124"/>
     </row>
     <row r="72" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A72" s="108"/>
-      <c r="B72" s="108"/>
-      <c r="C72" s="108"/>
-      <c r="D72" s="108"/>
-      <c r="E72" s="108"/>
-      <c r="F72" s="108"/>
-      <c r="G72" s="108"/>
-      <c r="H72" s="108"/>
-      <c r="I72" s="108"/>
-      <c r="J72" s="108"/>
-      <c r="K72" s="108"/>
-      <c r="L72" s="108"/>
-      <c r="M72" s="108"/>
-      <c r="N72" s="108"/>
-      <c r="O72" s="108"/>
-      <c r="P72" s="108"/>
-      <c r="Q72" s="108"/>
+      <c r="A72" s="122"/>
+      <c r="B72" s="122"/>
+      <c r="C72" s="122"/>
+      <c r="D72" s="122"/>
+      <c r="E72" s="122"/>
+      <c r="F72" s="122"/>
+      <c r="G72" s="122"/>
+      <c r="H72" s="122"/>
+      <c r="I72" s="122"/>
+      <c r="J72" s="122"/>
+      <c r="K72" s="122"/>
+      <c r="L72" s="122"/>
+      <c r="M72" s="122"/>
+      <c r="N72" s="122"/>
+      <c r="O72" s="122"/>
+      <c r="P72" s="122"/>
+      <c r="Q72" s="122"/>
     </row>
     <row r="73" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A73" s="108" t="s">
+      <c r="A73" s="122" t="s">
         <v>165</v>
       </c>
-      <c r="B73" s="108"/>
-      <c r="C73" s="108"/>
-      <c r="D73" s="108"/>
-      <c r="E73" s="108"/>
-      <c r="F73" s="108"/>
-      <c r="G73" s="108"/>
-      <c r="H73" s="108"/>
-      <c r="I73" s="108"/>
-      <c r="J73" s="108"/>
-      <c r="K73" s="108"/>
-      <c r="L73" s="108"/>
-      <c r="M73" s="108"/>
-      <c r="N73" s="108"/>
-      <c r="O73" s="108"/>
-      <c r="P73" s="108"/>
-      <c r="Q73" s="108"/>
+      <c r="B73" s="122"/>
+      <c r="C73" s="122"/>
+      <c r="D73" s="122"/>
+      <c r="E73" s="122"/>
+      <c r="F73" s="122"/>
+      <c r="G73" s="122"/>
+      <c r="H73" s="122"/>
+      <c r="I73" s="122"/>
+      <c r="J73" s="122"/>
+      <c r="K73" s="122"/>
+      <c r="L73" s="122"/>
+      <c r="M73" s="122"/>
+      <c r="N73" s="122"/>
+      <c r="O73" s="122"/>
+      <c r="P73" s="122"/>
+      <c r="Q73" s="122"/>
     </row>
     <row r="74" spans="1:17" ht="17.399999999999999" x14ac:dyDescent="0.25">
       <c r="A74" s="82"/>
@@ -4799,16 +4799,10 @@
   </sheetData>
   <autoFilter ref="A8:Q71"/>
   <mergeCells count="30">
-    <mergeCell ref="A1:Q1"/>
-    <mergeCell ref="A2:Q2"/>
-    <mergeCell ref="A3:Q3"/>
-    <mergeCell ref="C4:D4"/>
-    <mergeCell ref="E4:I4"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="A4:A8"/>
-    <mergeCell ref="B4:B8"/>
-    <mergeCell ref="C5:C8"/>
-    <mergeCell ref="D5:D8"/>
+    <mergeCell ref="A71:O71"/>
+    <mergeCell ref="E5:E8"/>
+    <mergeCell ref="F5:F8"/>
+    <mergeCell ref="A72:Q72"/>
     <mergeCell ref="A73:Q73"/>
     <mergeCell ref="G5:G8"/>
     <mergeCell ref="H5:H8"/>
@@ -4825,10 +4819,16 @@
     <mergeCell ref="O4:O8"/>
     <mergeCell ref="A69:O69"/>
     <mergeCell ref="A70:O70"/>
-    <mergeCell ref="A71:O71"/>
-    <mergeCell ref="E5:E8"/>
-    <mergeCell ref="F5:F8"/>
-    <mergeCell ref="A72:Q72"/>
+    <mergeCell ref="A1:Q1"/>
+    <mergeCell ref="A2:Q2"/>
+    <mergeCell ref="A3:Q3"/>
+    <mergeCell ref="C4:D4"/>
+    <mergeCell ref="E4:I4"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="A4:A8"/>
+    <mergeCell ref="B4:B8"/>
+    <mergeCell ref="C5:C8"/>
+    <mergeCell ref="D5:D8"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <pageMargins left="0.15902777777777799" right="0.16875000000000001" top="0.48888888888888898" bottom="0.31874999999999998" header="0.5" footer="0.5"/>

</xml_diff>